<commit_message>
Accession Register page code....
</commit_message>
<xml_diff>
--- a/IcamTestApplication/src/main/java/com/icam/qa/testdata/iCAM_Data_Sheet.xlsx
+++ b/IcamTestApplication/src/main/java/com/icam/qa/testdata/iCAM_Data_Sheet.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14235" windowHeight="3660" firstSheet="2" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15315" windowHeight="2595" firstSheet="38" activeTab="41"/>
   </bookViews>
   <sheets>
     <sheet name="Course" sheetId="1" r:id="rId1"/>
@@ -48,9 +48,10 @@
     <sheet name="CreateCategory" sheetId="39" r:id="rId39"/>
     <sheet name="TicketStatus" sheetId="40" r:id="rId40"/>
     <sheet name="TaskStatus" sheetId="41" r:id="rId41"/>
+    <sheet name="AccessionRegister" sheetId="43" r:id="rId42"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:M17"/>
+  <oleSize ref="A1:O6"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -60,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="258">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="268">
   <si>
     <t>CourseTypeName</t>
   </si>
@@ -834,6 +835,36 @@
   </si>
   <si>
     <t>XV</t>
+  </si>
+  <si>
+    <t>AccessionNo</t>
+  </si>
+  <si>
+    <t>Sources</t>
+  </si>
+  <si>
+    <t>WithdrawNo</t>
+  </si>
+  <si>
+    <t>Ac232</t>
+  </si>
+  <si>
+    <t>Steven</t>
+  </si>
+  <si>
+    <t>Europe</t>
+  </si>
+  <si>
+    <t>Wills</t>
+  </si>
+  <si>
+    <t>BL30</t>
+  </si>
+  <si>
+    <t>BK303</t>
+  </si>
+  <si>
+    <t>WD20</t>
   </si>
 </sst>
 </file>
@@ -2345,7 +2376,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
@@ -3011,6 +3042,118 @@
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>254</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="M2" sqref="M2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.42578125" customWidth="1"/>
+    <col min="2" max="2" width="23.140625" customWidth="1"/>
+    <col min="3" max="3" width="16.85546875" customWidth="1"/>
+    <col min="4" max="4" width="19.5703125" customWidth="1"/>
+    <col min="5" max="5" width="23.7109375" customWidth="1"/>
+    <col min="6" max="6" width="20.140625" customWidth="1"/>
+    <col min="7" max="7" width="19.140625" customWidth="1"/>
+    <col min="8" max="8" width="16.42578125" customWidth="1"/>
+    <col min="9" max="9" width="22.140625" customWidth="1"/>
+    <col min="10" max="10" width="17.85546875" customWidth="1"/>
+    <col min="11" max="11" width="19.5703125" customWidth="1"/>
+    <col min="12" max="12" width="22" customWidth="1"/>
+    <col min="13" max="13" width="20.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B1" t="s">
+        <v>258</v>
+      </c>
+      <c r="C1" t="s">
+        <v>97</v>
+      </c>
+      <c r="D1" t="s">
+        <v>103</v>
+      </c>
+      <c r="E1" t="s">
+        <v>105</v>
+      </c>
+      <c r="F1" t="s">
+        <v>93</v>
+      </c>
+      <c r="G1" t="s">
+        <v>95</v>
+      </c>
+      <c r="H1" t="s">
+        <v>259</v>
+      </c>
+      <c r="I1" t="s">
+        <v>104</v>
+      </c>
+      <c r="J1" t="s">
+        <v>94</v>
+      </c>
+      <c r="K1" t="s">
+        <v>96</v>
+      </c>
+      <c r="L1" t="s">
+        <v>99</v>
+      </c>
+      <c r="M1" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>165</v>
+      </c>
+      <c r="B2" t="s">
+        <v>261</v>
+      </c>
+      <c r="C2" t="s">
+        <v>262</v>
+      </c>
+      <c r="D2" t="s">
+        <v>263</v>
+      </c>
+      <c r="E2" t="s">
+        <v>264</v>
+      </c>
+      <c r="F2">
+        <v>2018</v>
+      </c>
+      <c r="G2">
+        <v>200</v>
+      </c>
+      <c r="H2" t="s">
+        <v>109</v>
+      </c>
+      <c r="I2" t="s">
+        <v>265</v>
+      </c>
+      <c r="J2">
+        <v>400</v>
+      </c>
+      <c r="K2">
+        <v>3</v>
+      </c>
+      <c r="L2" t="s">
+        <v>266</v>
+      </c>
+      <c r="M2" t="s">
+        <v>267</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add Create Event Page Code....
</commit_message>
<xml_diff>
--- a/IcamTestApplication/src/main/java/com/icam/qa/testdata/iCAM_Data_Sheet.xlsx
+++ b/IcamTestApplication/src/main/java/com/icam/qa/testdata/iCAM_Data_Sheet.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15315" windowHeight="2595" firstSheet="38" activeTab="41"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15480" windowHeight="3210" firstSheet="39" activeTab="42"/>
   </bookViews>
   <sheets>
     <sheet name="Course" sheetId="1" r:id="rId1"/>
@@ -49,9 +49,10 @@
     <sheet name="TicketStatus" sheetId="40" r:id="rId40"/>
     <sheet name="TaskStatus" sheetId="41" r:id="rId41"/>
     <sheet name="AccessionRegister" sheetId="43" r:id="rId42"/>
+    <sheet name="CreateEvent" sheetId="44" r:id="rId43"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:O6"/>
+  <oleSize ref="A1:O8"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -61,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="268">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="271">
   <si>
     <t>CourseTypeName</t>
   </si>
@@ -865,6 +866,15 @@
   </si>
   <si>
     <t>WD20</t>
+  </si>
+  <si>
+    <t>EventName</t>
+  </si>
+  <si>
+    <t>Incharge</t>
+  </si>
+  <si>
+    <t>Testing</t>
   </si>
 </sst>
 </file>
@@ -3053,7 +3063,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
@@ -3154,6 +3164,48 @@
       </c>
       <c r="M2" t="s">
         <v>267</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.5703125" customWidth="1"/>
+    <col min="2" max="2" width="32" customWidth="1"/>
+    <col min="3" max="3" width="21.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>268</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B2" t="s">
+        <v>270</v>
+      </c>
+      <c r="C2" t="s">
+        <v>57</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated code for event creation
</commit_message>
<xml_diff>
--- a/IcamTestApplication/src/main/java/com/icam/qa/testdata/iCAM_Data_Sheet.xlsx
+++ b/IcamTestApplication/src/main/java/com/icam/qa/testdata/iCAM_Data_Sheet.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15480" windowHeight="3210" firstSheet="39" activeTab="42"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15480" windowHeight="3000" firstSheet="39" activeTab="42"/>
   </bookViews>
   <sheets>
     <sheet name="Course" sheetId="1" r:id="rId1"/>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="271">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="381" uniqueCount="273">
   <si>
     <t>CourseTypeName</t>
   </si>
@@ -875,6 +875,12 @@
   </si>
   <si>
     <t>Testing</t>
+  </si>
+  <si>
+    <t>Auto</t>
+  </si>
+  <si>
+    <t>At</t>
   </si>
 </sst>
 </file>
@@ -3173,10 +3179,10 @@
 
 <file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3206,6 +3212,17 @@
       </c>
       <c r="C2" t="s">
         <v>57</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>271</v>
+      </c>
+      <c r="B3" t="s">
+        <v>272</v>
+      </c>
+      <c r="C3" t="s">
+        <v>131</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Student Achievement Page Added....
</commit_message>
<xml_diff>
--- a/IcamTestApplication/src/main/java/com/icam/qa/testdata/iCAM_Data_Sheet.xlsx
+++ b/IcamTestApplication/src/main/java/com/icam/qa/testdata/iCAM_Data_Sheet.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15480" windowHeight="3000" firstSheet="39" activeTab="42"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15240" windowHeight="2805" firstSheet="41" activeTab="43"/>
   </bookViews>
   <sheets>
     <sheet name="Course" sheetId="1" r:id="rId1"/>
@@ -50,9 +50,10 @@
     <sheet name="TaskStatus" sheetId="41" r:id="rId41"/>
     <sheet name="AccessionRegister" sheetId="43" r:id="rId42"/>
     <sheet name="CreateEvent" sheetId="44" r:id="rId43"/>
+    <sheet name="StudentAchievement" sheetId="45" r:id="rId44"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:O8"/>
+  <oleSize ref="A1:O7"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -62,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="381" uniqueCount="273">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="385" uniqueCount="277">
   <si>
     <t>CourseTypeName</t>
   </si>
@@ -881,6 +882,18 @@
   </si>
   <si>
     <t>At</t>
+  </si>
+  <si>
+    <t>EventPosition</t>
+  </si>
+  <si>
+    <t>Student</t>
+  </si>
+  <si>
+    <t>DevOpps</t>
+  </si>
+  <si>
+    <t>99999</t>
   </si>
 </sst>
 </file>
@@ -3181,7 +3194,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
@@ -3223,6 +3236,41 @@
       </c>
       <c r="C3" t="s">
         <v>131</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet44.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.140625" customWidth="1"/>
+    <col min="2" max="2" width="23.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>273</v>
+      </c>
+      <c r="B1" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>275</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>276</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Venue Allocation Page Added....
</commit_message>
<xml_diff>
--- a/IcamTestApplication/src/main/java/com/icam/qa/testdata/iCAM_Data_Sheet.xlsx
+++ b/IcamTestApplication/src/main/java/com/icam/qa/testdata/iCAM_Data_Sheet.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15240" windowHeight="2910" firstSheet="44" activeTab="45"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15240" windowHeight="2595" firstSheet="23" activeTab="24"/>
   </bookViews>
   <sheets>
     <sheet name="Course" sheetId="1" r:id="rId1"/>
@@ -55,7 +55,7 @@
     <sheet name="Facility" sheetId="47" r:id="rId46"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:O7"/>
+  <oleSize ref="A1:I6"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -2164,7 +2164,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
@@ -3348,7 +3348,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Create Ledger Page Added.....
</commit_message>
<xml_diff>
--- a/IcamTestApplication/src/main/java/com/icam/qa/testdata/iCAM_Data_Sheet.xlsx
+++ b/IcamTestApplication/src/main/java/com/icam/qa/testdata/iCAM_Data_Sheet.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15240" windowHeight="2595" firstSheet="23" activeTab="24"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15240" windowHeight="2625" firstSheet="44" activeTab="46"/>
   </bookViews>
   <sheets>
     <sheet name="Course" sheetId="1" r:id="rId1"/>
@@ -53,9 +53,10 @@
     <sheet name="StudentAchievement" sheetId="45" r:id="rId44"/>
     <sheet name="BookCatalogingAnd AccessionReg" sheetId="46" r:id="rId45"/>
     <sheet name="Facility" sheetId="47" r:id="rId46"/>
+    <sheet name="Ledger" sheetId="48" r:id="rId47"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:I6"/>
+  <oleSize ref="A1:O6"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -65,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="397" uniqueCount="282">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="401" uniqueCount="285">
   <si>
     <t>CourseTypeName</t>
   </si>
@@ -911,6 +912,15 @@
   </si>
   <si>
     <t>Auto Testing</t>
+  </si>
+  <si>
+    <t>LedgerName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Testing </t>
+  </si>
+  <si>
+    <t>2000</t>
   </si>
 </sst>
 </file>
@@ -2164,7 +2174,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
@@ -3372,6 +3382,41 @@
       </c>
       <c r="B2" t="s">
         <v>281</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet47.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21.85546875" customWidth="1"/>
+    <col min="2" max="2" width="25.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>282</v>
+      </c>
+      <c r="B1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>283</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>284</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Chnages in 2 file....
</commit_message>
<xml_diff>
--- a/IcamTestApplication/src/main/java/com/icam/qa/testdata/iCAM_Data_Sheet.xlsx
+++ b/IcamTestApplication/src/main/java/com/icam/qa/testdata/iCAM_Data_Sheet.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15240" windowHeight="2625" firstSheet="44" activeTab="46"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15240" windowHeight="1320" firstSheet="44" activeTab="45"/>
   </bookViews>
   <sheets>
     <sheet name="Course" sheetId="1" r:id="rId1"/>
@@ -56,7 +56,7 @@
     <sheet name="Ledger" sheetId="48" r:id="rId47"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:O6"/>
+  <oleSize ref="A1:K2"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -66,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="401" uniqueCount="285">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="401" uniqueCount="286">
   <si>
     <t>CourseTypeName</t>
   </si>
@@ -911,9 +911,6 @@
     <t>3000</t>
   </si>
   <si>
-    <t>Auto Testing</t>
-  </si>
-  <si>
     <t>LedgerName</t>
   </si>
   <si>
@@ -921,6 +918,12 @@
   </si>
   <si>
     <t>2000</t>
+  </si>
+  <si>
+    <t>RPA</t>
+  </si>
+  <si>
+    <t>Robotic Automation Process</t>
   </si>
 </sst>
 </file>
@@ -3358,8 +3361,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3378,10 +3381,10 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>270</v>
+        <v>284</v>
       </c>
       <c r="B2" t="s">
-        <v>281</v>
+        <v>285</v>
       </c>
     </row>
   </sheetData>
@@ -3393,7 +3396,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
@@ -3405,7 +3408,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B1" t="s">
         <v>89</v>
@@ -3413,10 +3416,10 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>282</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>283</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>284</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changes in Facility Pages
</commit_message>
<xml_diff>
--- a/IcamTestApplication/src/main/java/com/icam/qa/testdata/iCAM_Data_Sheet.xlsx
+++ b/IcamTestApplication/src/main/java/com/icam/qa/testdata/iCAM_Data_Sheet.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15240" windowHeight="1320" firstSheet="44" activeTab="45"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15240" windowHeight="2310" firstSheet="44" activeTab="45"/>
   </bookViews>
   <sheets>
     <sheet name="Course" sheetId="1" r:id="rId1"/>
@@ -66,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="401" uniqueCount="286">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="403" uniqueCount="287">
   <si>
     <t>CourseTypeName</t>
   </si>
@@ -924,6 +924,9 @@
   </si>
   <si>
     <t>Robotic Automation Process</t>
+  </si>
+  <si>
+    <t>QTP HP</t>
   </si>
 </sst>
 </file>
@@ -3359,10 +3362,10 @@
 
 <file path=xl/worksheets/sheet46.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3385,6 +3388,14 @@
       </c>
       <c r="B2" t="s">
         <v>285</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>166</v>
+      </c>
+      <c r="B3" t="s">
+        <v>286</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Student creation and category reciepent.
</commit_message>
<xml_diff>
--- a/IcamTestApplication/src/main/java/com/icam/qa/testdata/iCAM_Data_Sheet.xlsx
+++ b/IcamTestApplication/src/main/java/com/icam/qa/testdata/iCAM_Data_Sheet.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14640" windowHeight="2340" firstSheet="45" activeTab="47"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15255" windowHeight="2145" firstSheet="4" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Course" sheetId="1" r:id="rId1"/>
@@ -57,7 +57,7 @@
     <sheet name="Residence" sheetId="49" r:id="rId48"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:N5"/>
+  <oleSize ref="A1:H5"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -67,7 +67,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="409" uniqueCount="291">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="391" uniqueCount="283">
   <si>
     <t>CourseTypeName</t>
   </si>
@@ -708,87 +708,12 @@
     <t>Level 4</t>
   </si>
   <si>
-    <t>RollNo</t>
-  </si>
-  <si>
-    <t>FatherFirstName</t>
-  </si>
-  <si>
-    <t>FatherLastName</t>
-  </si>
-  <si>
-    <t>MotherFirstName</t>
-  </si>
-  <si>
-    <t>MotherLastName</t>
-  </si>
-  <si>
-    <t>GuardianLName</t>
-  </si>
-  <si>
-    <t>GuardianFName</t>
-  </si>
-  <si>
-    <t>Pincode</t>
-  </si>
-  <si>
-    <t>District</t>
-  </si>
-  <si>
-    <t>PostOffice</t>
-  </si>
-  <si>
-    <t>PoliceStation</t>
-  </si>
-  <si>
-    <t>GuardianLAddress</t>
-  </si>
-  <si>
-    <t>Guardian City</t>
-  </si>
-  <si>
-    <t>GuardianPincode</t>
-  </si>
-  <si>
-    <t>Post Office</t>
-  </si>
-  <si>
-    <t>PolicsStation</t>
-  </si>
-  <si>
-    <t>PersonalIdentification</t>
-  </si>
-  <si>
-    <t>Hyderabad</t>
-  </si>
-  <si>
-    <t>Falaknuma</t>
-  </si>
-  <si>
-    <t>Falakhnuma</t>
-  </si>
-  <si>
-    <t>None</t>
-  </si>
-  <si>
-    <t>500032</t>
-  </si>
-  <si>
     <t>Amit</t>
   </si>
   <si>
     <t>Mehra</t>
   </si>
   <si>
-    <t>sandip</t>
-  </si>
-  <si>
-    <t>mehra</t>
-  </si>
-  <si>
-    <t>puja</t>
-  </si>
-  <si>
     <t>1001</t>
   </si>
   <si>
@@ -940,6 +865,57 @@
   </si>
   <si>
     <t>Funct</t>
+  </si>
+  <si>
+    <t>SchoolNo</t>
+  </si>
+  <si>
+    <t>MiddleName</t>
+  </si>
+  <si>
+    <t>Hindu</t>
+  </si>
+  <si>
+    <t>MotherTongue</t>
+  </si>
+  <si>
+    <t>AadharNo</t>
+  </si>
+  <si>
+    <t>90929099029</t>
+  </si>
+  <si>
+    <t>Mobile</t>
+  </si>
+  <si>
+    <t>917575757575</t>
+  </si>
+  <si>
+    <t>SchoolName</t>
+  </si>
+  <si>
+    <t>Modern High</t>
+  </si>
+  <si>
+    <t>Website</t>
+  </si>
+  <si>
+    <t>ww.mdnhg.com</t>
+  </si>
+  <si>
+    <t>Ballygung Phari</t>
+  </si>
+  <si>
+    <t>918080808080</t>
+  </si>
+  <si>
+    <t>mdn@gmail</t>
+  </si>
+  <si>
+    <t>Achievement</t>
+  </si>
+  <si>
+    <t>Medal</t>
   </si>
 </sst>
 </file>
@@ -2360,22 +2336,22 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>241</v>
+        <v>216</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>242</v>
+        <v>217</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>243</v>
+        <v>218</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>244</v>
+        <v>219</v>
       </c>
     </row>
   </sheetData>
@@ -2471,7 +2447,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>255</v>
+        <v>230</v>
       </c>
       <c r="B2" t="s">
         <v>8</v>
@@ -2479,7 +2455,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>256</v>
+        <v>231</v>
       </c>
       <c r="B3" t="s">
         <v>8</v>
@@ -2487,7 +2463,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>257</v>
+        <v>232</v>
       </c>
       <c r="B4" t="s">
         <v>8</v>
@@ -2883,7 +2859,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>245</v>
+        <v>220</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
@@ -2928,16 +2904,16 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>246</v>
+        <v>221</v>
       </c>
       <c r="B2" t="s">
-        <v>247</v>
+        <v>222</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>248</v>
+        <v>223</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>249</v>
+        <v>224</v>
       </c>
     </row>
   </sheetData>
@@ -2965,13 +2941,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>250</v>
+        <v>225</v>
       </c>
       <c r="B1" t="s">
-        <v>251</v>
+        <v>226</v>
       </c>
       <c r="C1" t="s">
-        <v>252</v>
+        <v>227</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -3093,7 +3069,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>253</v>
+        <v>228</v>
       </c>
     </row>
   </sheetData>
@@ -3116,7 +3092,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>254</v>
+        <v>229</v>
       </c>
     </row>
   </sheetData>
@@ -3154,7 +3130,7 @@
         <v>100</v>
       </c>
       <c r="B1" t="s">
-        <v>258</v>
+        <v>233</v>
       </c>
       <c r="C1" t="s">
         <v>97</v>
@@ -3172,7 +3148,7 @@
         <v>95</v>
       </c>
       <c r="H1" t="s">
-        <v>259</v>
+        <v>234</v>
       </c>
       <c r="I1" t="s">
         <v>104</v>
@@ -3187,7 +3163,7 @@
         <v>99</v>
       </c>
       <c r="M1" t="s">
-        <v>260</v>
+        <v>235</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
@@ -3195,16 +3171,16 @@
         <v>165</v>
       </c>
       <c r="B2" t="s">
-        <v>261</v>
+        <v>236</v>
       </c>
       <c r="C2" t="s">
-        <v>262</v>
+        <v>237</v>
       </c>
       <c r="D2" t="s">
-        <v>263</v>
+        <v>238</v>
       </c>
       <c r="E2" t="s">
-        <v>264</v>
+        <v>239</v>
       </c>
       <c r="F2">
         <v>2018</v>
@@ -3216,7 +3192,7 @@
         <v>109</v>
       </c>
       <c r="I2" t="s">
-        <v>265</v>
+        <v>240</v>
       </c>
       <c r="J2">
         <v>400</v>
@@ -3225,10 +3201,10 @@
         <v>3</v>
       </c>
       <c r="L2" t="s">
-        <v>266</v>
+        <v>241</v>
       </c>
       <c r="M2" t="s">
-        <v>267</v>
+        <v>242</v>
       </c>
     </row>
   </sheetData>
@@ -3253,13 +3229,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>268</v>
+        <v>243</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>269</v>
+        <v>244</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -3267,7 +3243,7 @@
         <v>57</v>
       </c>
       <c r="B2" t="s">
-        <v>270</v>
+        <v>245</v>
       </c>
       <c r="C2" t="s">
         <v>57</v>
@@ -3275,10 +3251,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>271</v>
+        <v>246</v>
       </c>
       <c r="B3" t="s">
-        <v>272</v>
+        <v>247</v>
       </c>
       <c r="C3" t="s">
         <v>131</v>
@@ -3305,18 +3281,18 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>273</v>
+        <v>248</v>
       </c>
       <c r="B1" t="s">
-        <v>274</v>
+        <v>249</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>275</v>
+        <v>250</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>276</v>
+        <v>251</v>
       </c>
     </row>
   </sheetData>
@@ -3345,7 +3321,7 @@
         <v>100</v>
       </c>
       <c r="B1" t="s">
-        <v>258</v>
+        <v>233</v>
       </c>
       <c r="C1" t="s">
         <v>97</v>
@@ -3356,16 +3332,16 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>277</v>
+        <v>252</v>
       </c>
       <c r="B2" t="s">
-        <v>278</v>
+        <v>253</v>
       </c>
       <c r="C2" t="s">
-        <v>279</v>
+        <v>254</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>280</v>
+        <v>255</v>
       </c>
     </row>
   </sheetData>
@@ -3397,10 +3373,10 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>284</v>
+        <v>259</v>
       </c>
       <c r="B2" t="s">
-        <v>285</v>
+        <v>260</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -3408,7 +3384,7 @@
         <v>166</v>
       </c>
       <c r="B3" t="s">
-        <v>286</v>
+        <v>261</v>
       </c>
     </row>
   </sheetData>
@@ -3432,7 +3408,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>281</v>
+        <v>256</v>
       </c>
       <c r="B1" t="s">
         <v>89</v>
@@ -3440,10 +3416,10 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>282</v>
+        <v>257</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>283</v>
+        <v>258</v>
       </c>
     </row>
   </sheetData>
@@ -3455,7 +3431,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
@@ -3468,24 +3444,24 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>287</v>
+        <v>262</v>
       </c>
       <c r="B1" t="s">
-        <v>288</v>
+        <v>263</v>
       </c>
       <c r="C1" t="s">
-        <v>289</v>
+        <v>264</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>270</v>
+        <v>245</v>
       </c>
       <c r="B2" t="s">
         <v>136</v>
       </c>
       <c r="C2" t="s">
-        <v>290</v>
+        <v>265</v>
       </c>
     </row>
   </sheetData>
@@ -3495,179 +3471,120 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:X2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+  <dimension ref="A1:Y2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="N3" sqref="N3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.5703125" customWidth="1"/>
-    <col min="2" max="2" width="17.140625" customWidth="1"/>
-    <col min="3" max="3" width="22.140625" customWidth="1"/>
-    <col min="4" max="4" width="17.42578125" customWidth="1"/>
-    <col min="5" max="6" width="19.5703125" customWidth="1"/>
-    <col min="7" max="8" width="20.140625" customWidth="1"/>
-    <col min="9" max="9" width="18.42578125" customWidth="1"/>
-    <col min="10" max="10" width="19.42578125" customWidth="1"/>
-    <col min="11" max="11" width="23.140625" customWidth="1"/>
-    <col min="12" max="12" width="15.28515625" customWidth="1"/>
-    <col min="14" max="14" width="22.85546875" customWidth="1"/>
-    <col min="15" max="15" width="18.7109375" customWidth="1"/>
-    <col min="16" max="16" width="20.140625" customWidth="1"/>
-    <col min="17" max="17" width="21.7109375" customWidth="1"/>
-    <col min="18" max="18" width="17.28515625" customWidth="1"/>
-    <col min="19" max="19" width="23.28515625" customWidth="1"/>
-    <col min="20" max="20" width="22.85546875" customWidth="1"/>
-    <col min="21" max="21" width="19.5703125" customWidth="1"/>
-    <col min="22" max="22" width="20.85546875" customWidth="1"/>
-    <col min="23" max="23" width="26.5703125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>213</v>
+    <col min="2" max="3" width="17.140625" customWidth="1"/>
+    <col min="4" max="4" width="22.140625" customWidth="1"/>
+    <col min="5" max="5" width="13.28515625" customWidth="1"/>
+    <col min="6" max="6" width="20.7109375" customWidth="1"/>
+    <col min="7" max="8" width="20" customWidth="1"/>
+    <col min="9" max="9" width="30.7109375" customWidth="1"/>
+    <col min="10" max="10" width="24.42578125" customWidth="1"/>
+    <col min="11" max="11" width="26.5703125" customWidth="1"/>
+    <col min="12" max="12" width="19.140625" customWidth="1"/>
+    <col min="13" max="13" width="25.85546875" customWidth="1"/>
+    <col min="14" max="14" width="30.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>266</v>
       </c>
       <c r="B1" t="s">
         <v>29</v>
       </c>
       <c r="C1" t="s">
+        <v>267</v>
+      </c>
+      <c r="D1" t="s">
         <v>30</v>
       </c>
-      <c r="D1" t="s">
-        <v>35</v>
-      </c>
       <c r="E1" t="s">
-        <v>214</v>
+        <v>34</v>
       </c>
       <c r="F1" t="s">
-        <v>215</v>
+        <v>269</v>
       </c>
       <c r="G1" t="s">
-        <v>216</v>
+        <v>270</v>
       </c>
       <c r="H1" t="s">
-        <v>217</v>
+        <v>272</v>
       </c>
       <c r="I1" t="s">
-        <v>219</v>
+        <v>274</v>
       </c>
       <c r="J1" t="s">
-        <v>218</v>
+        <v>276</v>
       </c>
       <c r="K1" t="s">
         <v>38</v>
       </c>
       <c r="L1" t="s">
-        <v>39</v>
+        <v>266</v>
       </c>
       <c r="M1" t="s">
-        <v>220</v>
+        <v>33</v>
       </c>
       <c r="N1" t="s">
-        <v>221</v>
-      </c>
-      <c r="O1" t="s">
-        <v>222</v>
-      </c>
-      <c r="P1" t="s">
-        <v>223</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>224</v>
-      </c>
-      <c r="R1" t="s">
-        <v>225</v>
-      </c>
-      <c r="S1" t="s">
-        <v>226</v>
-      </c>
-      <c r="T1" t="s">
-        <v>221</v>
-      </c>
-      <c r="U1" t="s">
-        <v>227</v>
-      </c>
-      <c r="V1" t="s">
-        <v>228</v>
-      </c>
-      <c r="W1" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>240</v>
+        <v>215</v>
       </c>
       <c r="B2" t="s">
-        <v>235</v>
+        <v>213</v>
       </c>
       <c r="C2" t="s">
-        <v>236</v>
+        <v>213</v>
       </c>
       <c r="D2" t="s">
-        <v>46</v>
+        <v>214</v>
       </c>
       <c r="E2" t="s">
-        <v>237</v>
+        <v>268</v>
       </c>
       <c r="F2" t="s">
-        <v>238</v>
-      </c>
-      <c r="G2" t="s">
-        <v>239</v>
-      </c>
-      <c r="H2" t="s">
-        <v>238</v>
+        <v>47</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>273</v>
       </c>
       <c r="I2" t="s">
-        <v>237</v>
+        <v>275</v>
       </c>
       <c r="J2" t="s">
-        <v>238</v>
+        <v>277</v>
       </c>
       <c r="K2" t="s">
-        <v>231</v>
-      </c>
-      <c r="L2" t="s">
-        <v>230</v>
-      </c>
-      <c r="M2" s="2" t="s">
-        <v>234</v>
+        <v>278</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>279</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>280</v>
       </c>
       <c r="N2" t="s">
-        <v>230</v>
-      </c>
-      <c r="O2" t="s">
-        <v>232</v>
-      </c>
-      <c r="P2" t="s">
-        <v>232</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>232</v>
-      </c>
-      <c r="R2" t="s">
-        <v>230</v>
-      </c>
-      <c r="S2" s="2" t="s">
-        <v>234</v>
-      </c>
-      <c r="T2" t="s">
-        <v>230</v>
-      </c>
-      <c r="U2" t="s">
-        <v>232</v>
-      </c>
-      <c r="V2" t="s">
-        <v>232</v>
-      </c>
-      <c r="W2" t="s">
-        <v>233</v>
-      </c>
-    </row>
-  </sheetData>
+        <v>282</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="M2" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Task Status changes added
</commit_message>
<xml_diff>
--- a/IcamTestApplication/src/main/java/com/icam/qa/testdata/iCAM_Data_Sheet.xlsx
+++ b/IcamTestApplication/src/main/java/com/icam/qa/testdata/iCAM_Data_Sheet.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15255" windowHeight="2145" firstSheet="4" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14715" windowHeight="4200" firstSheet="37" activeTab="40"/>
   </bookViews>
   <sheets>
     <sheet name="Course" sheetId="1" r:id="rId1"/>
@@ -57,7 +57,7 @@
     <sheet name="Residence" sheetId="49" r:id="rId48"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:H5"/>
+  <oleSize ref="A1:M12"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -67,7 +67,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="391" uniqueCount="283">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="284">
   <si>
     <t>CourseTypeName</t>
   </si>
@@ -916,6 +916,9 @@
   </si>
   <si>
     <t>Medal</t>
+  </si>
+  <si>
+    <t>Open</t>
   </si>
 </sst>
 </file>
@@ -2929,7 +2932,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3079,10 +3082,10 @@
 
 <file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3093,6 +3096,11 @@
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>229</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>283</v>
       </c>
     </row>
   </sheetData>
@@ -3473,7 +3481,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="N3" sqref="N3"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Ticket Status changes added
</commit_message>
<xml_diff>
--- a/IcamTestApplication/src/main/java/com/icam/qa/testdata/iCAM_Data_Sheet.xlsx
+++ b/IcamTestApplication/src/main/java/com/icam/qa/testdata/iCAM_Data_Sheet.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14715" windowHeight="4200" firstSheet="37" activeTab="40"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14715" windowHeight="2415" firstSheet="37" activeTab="39"/>
   </bookViews>
   <sheets>
     <sheet name="Course" sheetId="1" r:id="rId1"/>
@@ -57,7 +57,7 @@
     <sheet name="Residence" sheetId="49" r:id="rId48"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:M12"/>
+  <oleSize ref="A1:M6"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -67,7 +67,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="284">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="393" uniqueCount="285">
   <si>
     <t>CourseTypeName</t>
   </si>
@@ -919,6 +919,9 @@
   </si>
   <si>
     <t>Open</t>
+  </si>
+  <si>
+    <t>WIP</t>
   </si>
 </sst>
 </file>
@@ -3059,9 +3062,9 @@
 
 <file path=xl/worksheets/sheet40.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -3075,6 +3078,11 @@
         <v>228</v>
       </c>
     </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>284</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3084,7 +3092,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Employee Details changes added...
</commit_message>
<xml_diff>
--- a/IcamTestApplication/src/main/java/com/icam/qa/testdata/iCAM_Data_Sheet.xlsx
+++ b/IcamTestApplication/src/main/java/com/icam/qa/testdata/iCAM_Data_Sheet.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14715" windowHeight="2415" firstSheet="37" activeTab="39"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14715" windowHeight="2415" firstSheet="11" activeTab="12"/>
   </bookViews>
   <sheets>
     <sheet name="Course" sheetId="1" r:id="rId1"/>
@@ -57,7 +57,7 @@
     <sheet name="Residence" sheetId="49" r:id="rId48"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:M6"/>
+  <oleSize ref="H1:O6"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -67,7 +67,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="393" uniqueCount="285">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="373" uniqueCount="272">
   <si>
     <t>CourseTypeName</t>
   </si>
@@ -177,78 +177,36 @@
     <t>Nationality</t>
   </si>
   <si>
-    <t>Language</t>
-  </si>
-  <si>
-    <t>FFirstName</t>
-  </si>
-  <si>
     <t>Address</t>
   </si>
   <si>
     <t>City</t>
   </si>
   <si>
-    <t>PinCode</t>
-  </si>
-  <si>
-    <t>EmployeeCode</t>
-  </si>
-  <si>
     <t>Rehan</t>
   </si>
   <si>
     <t>Abrahim</t>
   </si>
   <si>
-    <t>rehan@gmail.com</t>
-  </si>
-  <si>
-    <t>Islam</t>
-  </si>
-  <si>
     <t>Indian</t>
   </si>
   <si>
     <t>Hindi</t>
   </si>
   <si>
-    <t>Abdul</t>
-  </si>
-  <si>
-    <t>Wahid</t>
-  </si>
-  <si>
     <t>Park Street</t>
   </si>
   <si>
     <t>Kolkata</t>
   </si>
   <si>
-    <t>EMP2002</t>
-  </si>
-  <si>
-    <t>MFirstName</t>
-  </si>
-  <si>
-    <t>MLastName</t>
-  </si>
-  <si>
-    <t>FLastName</t>
-  </si>
-  <si>
     <t>DesignationType</t>
   </si>
   <si>
     <t>Test</t>
   </si>
   <si>
-    <t>M</t>
-  </si>
-  <si>
-    <t>L</t>
-  </si>
-  <si>
     <t>Designation Name</t>
   </si>
   <si>
@@ -573,9 +531,6 @@
     <t>9051496634</t>
   </si>
   <si>
-    <t>700016</t>
-  </si>
-  <si>
     <t>HighestQualification</t>
   </si>
   <si>
@@ -922,6 +877,12 @@
   </si>
   <si>
     <t>WIP</t>
+  </si>
+  <si>
+    <t>UserId</t>
+  </si>
+  <si>
+    <t>EMP8001</t>
   </si>
 </sst>
 </file>
@@ -1312,17 +1273,17 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>166</v>
+        <v>152</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>61</v>
+        <v>47</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>165</v>
+        <v>151</v>
       </c>
     </row>
   </sheetData>
@@ -1362,16 +1323,16 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>153</v>
+        <v>139</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>150</v>
+        <v>136</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>154</v>
+        <v>140</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>155</v>
+        <v>141</v>
       </c>
     </row>
   </sheetData>
@@ -1399,7 +1360,7 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>156</v>
+        <v>142</v>
       </c>
     </row>
   </sheetData>
@@ -1411,8 +1372,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R2"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="Q1" sqref="Q1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1420,16 +1381,8 @@
     <col min="1" max="1" width="21.28515625" customWidth="1"/>
     <col min="2" max="2" width="15.7109375" customWidth="1"/>
     <col min="3" max="3" width="15.5703125" customWidth="1"/>
-    <col min="4" max="5" width="19.28515625" customWidth="1"/>
-    <col min="6" max="6" width="17.85546875" customWidth="1"/>
-    <col min="7" max="7" width="17.42578125" customWidth="1"/>
-    <col min="8" max="8" width="18" customWidth="1"/>
-    <col min="9" max="9" width="16.5703125" customWidth="1"/>
-    <col min="10" max="12" width="14.5703125" customWidth="1"/>
-    <col min="13" max="13" width="16.85546875" customWidth="1"/>
-    <col min="14" max="14" width="17.42578125" customWidth="1"/>
-    <col min="15" max="15" width="16.42578125" customWidth="1"/>
-    <col min="16" max="16" width="18.140625" customWidth="1"/>
+    <col min="4" max="4" width="19.28515625" customWidth="1"/>
+    <col min="5" max="5" width="17.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.25">
@@ -1446,126 +1399,63 @@
         <v>32</v>
       </c>
       <c r="E1" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="F1" t="s">
-        <v>34</v>
-      </c>
-      <c r="G1" t="s">
-        <v>35</v>
-      </c>
-      <c r="H1" t="s">
-        <v>36</v>
-      </c>
-      <c r="I1" t="s">
-        <v>37</v>
-      </c>
-      <c r="J1" t="s">
-        <v>55</v>
-      </c>
-      <c r="K1" t="s">
-        <v>53</v>
-      </c>
-      <c r="L1" t="s">
-        <v>54</v>
-      </c>
-      <c r="M1" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>38</v>
       </c>
-      <c r="N1" t="s">
+      <c r="B2" t="s">
         <v>39</v>
       </c>
-      <c r="O1" t="s">
+      <c r="C2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="E2" t="s">
         <v>40</v>
       </c>
-      <c r="P1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>42</v>
-      </c>
-      <c r="B2" t="s">
-        <v>43</v>
-      </c>
-      <c r="C2" t="s">
-        <v>42</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>167</v>
-      </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" t="s">
+        <v>271</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
         <v>44</v>
       </c>
-      <c r="F2" t="s">
-        <v>45</v>
-      </c>
-      <c r="G2" t="s">
-        <v>46</v>
-      </c>
-      <c r="H2" t="s">
-        <v>47</v>
-      </c>
-      <c r="I2" t="s">
-        <v>48</v>
-      </c>
-      <c r="J2" t="s">
-        <v>49</v>
-      </c>
-      <c r="K2" t="s">
-        <v>58</v>
-      </c>
-      <c r="L2" t="s">
-        <v>59</v>
-      </c>
-      <c r="M2" t="s">
-        <v>50</v>
-      </c>
-      <c r="N2" t="s">
-        <v>51</v>
-      </c>
-      <c r="O2" s="2" t="s">
-        <v>168</v>
-      </c>
-      <c r="P2" t="s">
-        <v>52</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="21.140625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>56</v>
-      </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>180</v>
+        <v>165</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>181</v>
+        <v>166</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25"/>
@@ -1589,17 +1479,17 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>60</v>
+        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>178</v>
+        <v>163</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>179</v>
+        <v>164</v>
       </c>
     </row>
   </sheetData>
@@ -1622,17 +1512,17 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>62</v>
+        <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>211</v>
+        <v>196</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>212</v>
+        <v>197</v>
       </c>
     </row>
   </sheetData>
@@ -1655,45 +1545,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>81</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A7"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="17.85546875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>64</v>
+        <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
@@ -1711,19 +1563,57 @@
         <v>67</v>
       </c>
     </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>53</v>
+      </c>
+    </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>68</v>
+        <v>54</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>69</v>
+        <v>55</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>70</v>
+        <v>56</v>
       </c>
     </row>
   </sheetData>
@@ -1748,35 +1638,35 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>71</v>
+        <v>57</v>
       </c>
       <c r="B1" t="s">
-        <v>72</v>
+        <v>58</v>
       </c>
       <c r="C1" t="s">
-        <v>73</v>
+        <v>59</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>74</v>
+        <v>60</v>
       </c>
       <c r="B2" t="s">
-        <v>75</v>
+        <v>61</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>151</v>
+        <v>137</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>76</v>
+        <v>62</v>
       </c>
       <c r="B3" t="s">
-        <v>77</v>
+        <v>63</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>152</v>
+        <v>138</v>
       </c>
     </row>
   </sheetData>
@@ -1801,10 +1691,10 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>71</v>
+        <v>57</v>
       </c>
       <c r="B1" t="s">
-        <v>183</v>
+        <v>168</v>
       </c>
       <c r="C1" t="s">
         <v>11</v>
@@ -1812,46 +1702,46 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>187</v>
+        <v>172</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>164</v>
+        <v>150</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>182</v>
+        <v>167</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>184</v>
+        <v>169</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>152</v>
+        <v>138</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>153</v>
+        <v>139</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>185</v>
+        <v>170</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>164</v>
+        <v>150</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>182</v>
+        <v>167</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>186</v>
+        <v>171</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>164</v>
+        <v>150</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>182</v>
+        <v>167</v>
       </c>
     </row>
   </sheetData>
@@ -1874,17 +1764,17 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>78</v>
+        <v>64</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>147</v>
+        <v>133</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>146</v>
+        <v>132</v>
       </c>
     </row>
   </sheetData>
@@ -1908,10 +1798,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>82</v>
+        <v>68</v>
       </c>
       <c r="B1" t="s">
-        <v>83</v>
+        <v>69</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -1948,45 +1838,45 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>84</v>
+        <v>70</v>
       </c>
       <c r="B1" t="s">
-        <v>85</v>
+        <v>71</v>
       </c>
       <c r="C1" t="s">
-        <v>86</v>
+        <v>72</v>
       </c>
       <c r="D1" t="s">
-        <v>87</v>
+        <v>73</v>
       </c>
       <c r="E1" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="F1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="G1" t="s">
-        <v>89</v>
+        <v>75</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>90</v>
+        <v>76</v>
       </c>
       <c r="B2" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="C2">
         <v>908098097657</v>
       </c>
       <c r="D2" t="s">
-        <v>91</v>
+        <v>77</v>
       </c>
       <c r="E2">
         <v>3212</v>
       </c>
       <c r="F2" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="G2">
         <v>100</v>
@@ -2024,46 +1914,46 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>93</v>
+        <v>79</v>
       </c>
       <c r="B1" t="s">
-        <v>94</v>
+        <v>80</v>
       </c>
       <c r="C1" t="s">
-        <v>95</v>
+        <v>81</v>
       </c>
       <c r="D1" t="s">
-        <v>96</v>
+        <v>82</v>
       </c>
       <c r="E1" t="s">
-        <v>97</v>
+        <v>83</v>
       </c>
       <c r="F1" t="s">
-        <v>98</v>
+        <v>84</v>
       </c>
       <c r="G1" t="s">
-        <v>99</v>
+        <v>85</v>
       </c>
       <c r="H1" t="s">
-        <v>100</v>
+        <v>86</v>
       </c>
       <c r="I1" t="s">
-        <v>101</v>
+        <v>87</v>
       </c>
       <c r="J1" t="s">
-        <v>102</v>
+        <v>88</v>
       </c>
       <c r="K1" t="s">
-        <v>103</v>
+        <v>89</v>
       </c>
       <c r="L1" t="s">
-        <v>104</v>
+        <v>90</v>
       </c>
       <c r="M1" t="s">
-        <v>105</v>
+        <v>91</v>
       </c>
       <c r="N1" t="s">
-        <v>106</v>
+        <v>92</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
@@ -2080,34 +1970,34 @@
         <v>2</v>
       </c>
       <c r="E2" t="s">
-        <v>112</v>
+        <v>98</v>
       </c>
       <c r="F2">
         <v>4</v>
       </c>
       <c r="G2" t="s">
-        <v>111</v>
+        <v>97</v>
       </c>
       <c r="H2" t="s">
-        <v>110</v>
+        <v>96</v>
       </c>
       <c r="I2" t="s">
-        <v>109</v>
+        <v>95</v>
       </c>
       <c r="J2">
         <v>21</v>
       </c>
       <c r="K2" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="L2">
         <v>121</v>
       </c>
       <c r="M2" t="s">
-        <v>108</v>
+        <v>94</v>
       </c>
       <c r="N2" t="s">
-        <v>107</v>
+        <v>93</v>
       </c>
     </row>
   </sheetData>
@@ -2134,33 +2024,33 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>113</v>
+        <v>99</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>114</v>
+        <v>100</v>
       </c>
       <c r="D1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E1" t="s">
-        <v>115</v>
+        <v>101</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>116</v>
+        <v>102</v>
       </c>
       <c r="B2" t="s">
-        <v>117</v>
+        <v>103</v>
       </c>
       <c r="C2" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="D2" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="E2">
         <v>700016</v>
@@ -2191,42 +2081,42 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>118</v>
+        <v>104</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>119</v>
+        <v>105</v>
       </c>
       <c r="D1" t="s">
-        <v>120</v>
+        <v>106</v>
       </c>
       <c r="E1" t="s">
-        <v>121</v>
+        <v>107</v>
       </c>
       <c r="F1" t="s">
-        <v>122</v>
+        <v>108</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>123</v>
+        <v>109</v>
       </c>
       <c r="B2" t="s">
-        <v>124</v>
+        <v>110</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>182</v>
+        <v>167</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>152</v>
+        <v>138</v>
       </c>
       <c r="E2" t="s">
-        <v>123</v>
+        <v>109</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>152</v>
+        <v>138</v>
       </c>
     </row>
   </sheetData>
@@ -2250,7 +2140,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>125</v>
+        <v>111</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
@@ -2258,10 +2148,10 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="B2" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -2286,35 +2176,35 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>159</v>
+        <v>145</v>
       </c>
       <c r="B1" t="s">
-        <v>160</v>
+        <v>146</v>
       </c>
       <c r="C1" t="s">
-        <v>161</v>
+        <v>147</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>162</v>
+        <v>148</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>164</v>
+        <v>150</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>164</v>
+        <v>150</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>163</v>
+        <v>149</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>164</v>
+        <v>150</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>164</v>
+        <v>150</v>
       </c>
     </row>
   </sheetData>
@@ -2337,27 +2227,27 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>126</v>
+        <v>112</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>216</v>
+        <v>201</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>217</v>
+        <v>202</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>218</v>
+        <v>203</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>219</v>
+        <v>204</v>
       </c>
     </row>
   </sheetData>
@@ -2382,46 +2272,46 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>127</v>
+        <v>113</v>
       </c>
       <c r="B1" t="s">
-        <v>128</v>
+        <v>114</v>
       </c>
       <c r="C1" t="s">
-        <v>129</v>
+        <v>115</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="B2" t="s">
-        <v>130</v>
+        <v>116</v>
       </c>
       <c r="C2" t="s">
-        <v>131</v>
+        <v>117</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>132</v>
+        <v>118</v>
       </c>
       <c r="B3" t="s">
-        <v>133</v>
+        <v>119</v>
       </c>
       <c r="C3" t="s">
-        <v>134</v>
+        <v>120</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>135</v>
+        <v>121</v>
       </c>
       <c r="B4" t="s">
-        <v>136</v>
+        <v>122</v>
       </c>
       <c r="C4" t="s">
-        <v>137</v>
+        <v>123</v>
       </c>
     </row>
   </sheetData>
@@ -2453,7 +2343,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>230</v>
+        <v>215</v>
       </c>
       <c r="B2" t="s">
         <v>8</v>
@@ -2461,7 +2351,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>231</v>
+        <v>216</v>
       </c>
       <c r="B3" t="s">
         <v>8</v>
@@ -2469,7 +2359,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>232</v>
+        <v>217</v>
       </c>
       <c r="B4" t="s">
         <v>8</v>
@@ -2500,7 +2390,7 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>138</v>
+        <v>124</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
@@ -2520,22 +2410,22 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>139</v>
+        <v>125</v>
       </c>
       <c r="B2" t="s">
-        <v>140</v>
+        <v>126</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>144</v>
+        <v>130</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>145</v>
+        <v>131</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>146</v>
+        <v>132</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>147</v>
+        <v>133</v>
       </c>
     </row>
   </sheetData>
@@ -2562,7 +2452,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>141</v>
+        <v>127</v>
       </c>
       <c r="B1" t="s">
         <v>19</v>
@@ -2579,19 +2469,19 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>142</v>
+        <v>128</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>143</v>
+        <v>129</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>144</v>
+        <v>130</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>145</v>
+        <v>131</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>146</v>
+        <v>132</v>
       </c>
     </row>
   </sheetData>
@@ -2616,24 +2506,24 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>120</v>
+        <v>106</v>
       </c>
       <c r="B1" t="s">
-        <v>148</v>
+        <v>134</v>
       </c>
       <c r="C1" t="s">
-        <v>82</v>
+        <v>68</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>150</v>
+        <v>136</v>
       </c>
       <c r="B2" t="s">
-        <v>149</v>
+        <v>135</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>151</v>
+        <v>137</v>
       </c>
     </row>
   </sheetData>
@@ -2665,24 +2555,24 @@
         <v>30</v>
       </c>
       <c r="C1" t="s">
-        <v>169</v>
+        <v>154</v>
       </c>
       <c r="D1" t="s">
-        <v>170</v>
+        <v>155</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>171</v>
+        <v>156</v>
       </c>
       <c r="B2" t="s">
-        <v>172</v>
+        <v>157</v>
       </c>
       <c r="C2" t="s">
-        <v>173</v>
+        <v>158</v>
       </c>
       <c r="D2" t="s">
-        <v>174</v>
+        <v>159</v>
       </c>
     </row>
   </sheetData>
@@ -2706,18 +2596,18 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>175</v>
+        <v>160</v>
       </c>
       <c r="B1" t="s">
-        <v>176</v>
+        <v>161</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>177</v>
+        <v>162</v>
       </c>
     </row>
   </sheetData>
@@ -2747,98 +2637,98 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>71</v>
+        <v>57</v>
       </c>
       <c r="B1" t="s">
-        <v>188</v>
+        <v>173</v>
       </c>
       <c r="C1" t="s">
         <v>33</v>
       </c>
       <c r="D1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E1" t="s">
-        <v>84</v>
+        <v>70</v>
       </c>
       <c r="F1" t="s">
-        <v>192</v>
+        <v>177</v>
       </c>
       <c r="G1" t="s">
-        <v>194</v>
+        <v>179</v>
       </c>
       <c r="H1" t="s">
-        <v>196</v>
+        <v>181</v>
       </c>
       <c r="I1" t="s">
-        <v>198</v>
+        <v>183</v>
       </c>
       <c r="J1" t="s">
-        <v>89</v>
+        <v>75</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>201</v>
+        <v>186</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>189</v>
+        <v>174</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>202</v>
+        <v>187</v>
       </c>
       <c r="D2" t="s">
-        <v>190</v>
+        <v>175</v>
       </c>
       <c r="E2" t="s">
-        <v>191</v>
+        <v>176</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>193</v>
+        <v>178</v>
       </c>
       <c r="G2" t="s">
-        <v>195</v>
+        <v>180</v>
       </c>
       <c r="H2" t="s">
-        <v>197</v>
+        <v>182</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>199</v>
+        <v>184</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>200</v>
+        <v>185</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>203</v>
+        <v>188</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>204</v>
+        <v>189</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>205</v>
+        <v>190</v>
       </c>
       <c r="D3" t="s">
-        <v>206</v>
+        <v>191</v>
       </c>
       <c r="E3" t="s">
-        <v>191</v>
+        <v>176</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>207</v>
+        <v>192</v>
       </c>
       <c r="G3" t="s">
-        <v>208</v>
+        <v>193</v>
       </c>
       <c r="H3" t="s">
-        <v>197</v>
+        <v>182</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>209</v>
+        <v>194</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>210</v>
+        <v>195</v>
       </c>
     </row>
   </sheetData>
@@ -2865,12 +2755,12 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>220</v>
+        <v>205</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>145</v>
+        <v>131</v>
       </c>
     </row>
   </sheetData>
@@ -2902,7 +2792,7 @@
         <v>30</v>
       </c>
       <c r="C1" t="s">
-        <v>188</v>
+        <v>173</v>
       </c>
       <c r="D1" t="s">
         <v>33</v>
@@ -2910,16 +2800,16 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>221</v>
+        <v>206</v>
       </c>
       <c r="B2" t="s">
-        <v>222</v>
+        <v>207</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>224</v>
+        <v>209</v>
       </c>
     </row>
   </sheetData>
@@ -2947,24 +2837,24 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>225</v>
+        <v>210</v>
       </c>
       <c r="B1" t="s">
-        <v>226</v>
+        <v>211</v>
       </c>
       <c r="C1" t="s">
-        <v>227</v>
+        <v>212</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="B2" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="C2" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -3024,13 +2914,13 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>157</v>
+        <v>143</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>150</v>
+        <v>136</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>182</v>
+        <v>167</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -3038,21 +2928,21 @@
         <v>9</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>150</v>
+        <v>136</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>182</v>
+        <v>167</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>158</v>
+        <v>144</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>150</v>
+        <v>136</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>182</v>
+        <v>167</v>
       </c>
     </row>
   </sheetData>
@@ -3064,7 +2954,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -3075,12 +2965,12 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>228</v>
+        <v>213</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>284</v>
+        <v>269</v>
       </c>
     </row>
   </sheetData>
@@ -3103,12 +2993,12 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>229</v>
+        <v>214</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>283</v>
+        <v>268</v>
       </c>
     </row>
   </sheetData>
@@ -3143,60 +3033,60 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>100</v>
+        <v>86</v>
       </c>
       <c r="B1" t="s">
-        <v>233</v>
+        <v>218</v>
       </c>
       <c r="C1" t="s">
-        <v>97</v>
+        <v>83</v>
       </c>
       <c r="D1" t="s">
-        <v>103</v>
+        <v>89</v>
       </c>
       <c r="E1" t="s">
-        <v>105</v>
+        <v>91</v>
       </c>
       <c r="F1" t="s">
-        <v>93</v>
+        <v>79</v>
       </c>
       <c r="G1" t="s">
-        <v>95</v>
+        <v>81</v>
       </c>
       <c r="H1" t="s">
-        <v>234</v>
+        <v>219</v>
       </c>
       <c r="I1" t="s">
-        <v>104</v>
+        <v>90</v>
       </c>
       <c r="J1" t="s">
-        <v>94</v>
+        <v>80</v>
       </c>
       <c r="K1" t="s">
-        <v>96</v>
+        <v>82</v>
       </c>
       <c r="L1" t="s">
-        <v>99</v>
+        <v>85</v>
       </c>
       <c r="M1" t="s">
-        <v>235</v>
+        <v>220</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>165</v>
+        <v>151</v>
       </c>
       <c r="B2" t="s">
-        <v>236</v>
+        <v>221</v>
       </c>
       <c r="C2" t="s">
-        <v>237</v>
+        <v>222</v>
       </c>
       <c r="D2" t="s">
-        <v>238</v>
+        <v>223</v>
       </c>
       <c r="E2" t="s">
-        <v>239</v>
+        <v>224</v>
       </c>
       <c r="F2">
         <v>2018</v>
@@ -3205,10 +3095,10 @@
         <v>200</v>
       </c>
       <c r="H2" t="s">
-        <v>109</v>
+        <v>95</v>
       </c>
       <c r="I2" t="s">
-        <v>240</v>
+        <v>225</v>
       </c>
       <c r="J2">
         <v>400</v>
@@ -3217,10 +3107,10 @@
         <v>3</v>
       </c>
       <c r="L2" t="s">
-        <v>241</v>
+        <v>226</v>
       </c>
       <c r="M2" t="s">
-        <v>242</v>
+        <v>227</v>
       </c>
     </row>
   </sheetData>
@@ -3245,35 +3135,35 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>243</v>
+        <v>228</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>244</v>
+        <v>229</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="B2" t="s">
-        <v>245</v>
+        <v>230</v>
       </c>
       <c r="C2" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>246</v>
+        <v>231</v>
       </c>
       <c r="B3" t="s">
-        <v>247</v>
+        <v>232</v>
       </c>
       <c r="C3" t="s">
-        <v>131</v>
+        <v>117</v>
       </c>
     </row>
   </sheetData>
@@ -3297,18 +3187,18 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>248</v>
+        <v>233</v>
       </c>
       <c r="B1" t="s">
-        <v>249</v>
+        <v>234</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>250</v>
+        <v>235</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>251</v>
+        <v>236</v>
       </c>
     </row>
   </sheetData>
@@ -3334,30 +3224,30 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>100</v>
+        <v>86</v>
       </c>
       <c r="B1" t="s">
-        <v>233</v>
+        <v>218</v>
       </c>
       <c r="C1" t="s">
-        <v>97</v>
+        <v>83</v>
       </c>
       <c r="D1" t="s">
-        <v>94</v>
+        <v>80</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>252</v>
+        <v>237</v>
       </c>
       <c r="B2" t="s">
-        <v>253</v>
+        <v>238</v>
       </c>
       <c r="C2" t="s">
-        <v>254</v>
+        <v>239</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>255</v>
+        <v>240</v>
       </c>
     </row>
   </sheetData>
@@ -3381,7 +3271,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>138</v>
+        <v>124</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
@@ -3389,18 +3279,18 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>259</v>
+        <v>244</v>
       </c>
       <c r="B2" t="s">
-        <v>260</v>
+        <v>245</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>166</v>
+        <v>152</v>
       </c>
       <c r="B3" t="s">
-        <v>261</v>
+        <v>246</v>
       </c>
     </row>
   </sheetData>
@@ -3424,18 +3314,18 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>256</v>
+        <v>241</v>
       </c>
       <c r="B1" t="s">
-        <v>89</v>
+        <v>75</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>257</v>
+        <v>242</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>258</v>
+        <v>243</v>
       </c>
     </row>
   </sheetData>
@@ -3460,24 +3350,24 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>262</v>
+        <v>247</v>
       </c>
       <c r="B1" t="s">
-        <v>263</v>
+        <v>248</v>
       </c>
       <c r="C1" t="s">
-        <v>264</v>
+        <v>249</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>245</v>
+        <v>230</v>
       </c>
       <c r="B2" t="s">
-        <v>136</v>
+        <v>122</v>
       </c>
       <c r="C2" t="s">
-        <v>265</v>
+        <v>250</v>
       </c>
     </row>
   </sheetData>
@@ -3511,13 +3401,13 @@
   <sheetData>
     <row r="1" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>266</v>
+        <v>251</v>
       </c>
       <c r="B1" t="s">
         <v>29</v>
       </c>
       <c r="C1" t="s">
-        <v>267</v>
+        <v>252</v>
       </c>
       <c r="D1" t="s">
         <v>30</v>
@@ -3526,75 +3416,75 @@
         <v>34</v>
       </c>
       <c r="F1" t="s">
-        <v>269</v>
+        <v>254</v>
       </c>
       <c r="G1" t="s">
-        <v>270</v>
+        <v>255</v>
       </c>
       <c r="H1" t="s">
-        <v>272</v>
+        <v>257</v>
       </c>
       <c r="I1" t="s">
-        <v>274</v>
+        <v>259</v>
       </c>
       <c r="J1" t="s">
-        <v>276</v>
+        <v>261</v>
       </c>
       <c r="K1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="L1" t="s">
-        <v>266</v>
+        <v>251</v>
       </c>
       <c r="M1" t="s">
         <v>33</v>
       </c>
       <c r="N1" t="s">
-        <v>281</v>
+        <v>266</v>
       </c>
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>215</v>
+        <v>200</v>
       </c>
       <c r="B2" t="s">
-        <v>213</v>
+        <v>198</v>
       </c>
       <c r="C2" t="s">
-        <v>213</v>
+        <v>198</v>
       </c>
       <c r="D2" t="s">
-        <v>214</v>
+        <v>199</v>
       </c>
       <c r="E2" t="s">
-        <v>268</v>
+        <v>253</v>
       </c>
       <c r="F2" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>271</v>
+        <v>256</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>273</v>
+        <v>258</v>
       </c>
       <c r="I2" t="s">
-        <v>275</v>
+        <v>260</v>
       </c>
       <c r="J2" t="s">
-        <v>277</v>
+        <v>262</v>
       </c>
       <c r="K2" t="s">
-        <v>278</v>
+        <v>263</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>279</v>
+        <v>264</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>280</v>
+        <v>265</v>
       </c>
       <c r="N2" t="s">
-        <v>282</v>
+        <v>267</v>
       </c>
     </row>
   </sheetData>

</xml_diff>